<commit_message>
Added File generation Functionaity
</commit_message>
<xml_diff>
--- a/FakeDataCreate/resources/Configuration.xlsx
+++ b/FakeDataCreate/resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GuruKrishna\git\FakeDataCreate\FakeDataCreate\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FC8260-B3BC-4399-B8AF-D26F136D913B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22368588-F6B0-43E3-8446-246F96EFAF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Configuration Attributes</t>
   </si>
@@ -64,37 +64,31 @@
     <t>Name_Of_File</t>
   </si>
   <si>
-    <t>Mandetory_Files</t>
-  </si>
-  <si>
-    <t>Optional_Files</t>
-  </si>
-  <si>
     <t>Only_Generate_Mandetory_Files</t>
   </si>
   <si>
+    <t>Valid</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Invalid</t>
-  </si>
-  <si>
-    <t>Mandetory</t>
+    <t>Optional</t>
   </si>
   <si>
     <t>InValidNameFilesInclude</t>
   </si>
   <si>
-    <t>MandetoryFiles</t>
-  </si>
-  <si>
     <t>Attributes</t>
   </si>
   <si>
     <t>Values</t>
   </si>
   <si>
-    <t>Contract|Instrument|CounterParty|ControlFile</t>
+    <t>This is Applicable when Name of File is Valid.</t>
+  </si>
+  <si>
+    <t>This is Applicable when Name of File is Invalid.</t>
   </si>
 </sst>
 </file>
@@ -146,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,22 +163,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -199,9 +182,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,18 +462,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -509,7 +490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -517,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -525,15 +506,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -541,7 +522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -549,7 +530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -557,75 +538,61 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{35BA4643-0BE6-4DA3-A616-2A7639C5A105}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B10" xr:uid="{35BA4643-0BE6-4DA3-A616-2A7639C5A105}">
       <formula1>"Valid,Invalid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B12 B3:B8" xr:uid="{C5C61E9C-0E3E-49C2-869F-869CAE4F5ACC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B8 B11" xr:uid="{C5C61E9C-0E3E-49C2-869F-869CAE4F5ACC}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{E1DC10D7-6DFA-4596-9793-99FDF81D8328}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{E1DC10D7-6DFA-4596-9793-99FDF81D8328}">
       <formula1>"Mandetory,Optional,Both"</formula1>
     </dataValidation>
   </dataValidations>
@@ -651,10 +618,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>